<commit_message>
Add analysis sheet for allgather
</commit_message>
<xml_diff>
--- a/sheets/GameofLife.xlsx
+++ b/sheets/GameofLife.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18840" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -316,11 +316,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1324474544"/>
-        <c:axId val="-1324470448"/>
+        <c:axId val="1886701568"/>
+        <c:axId val="1886704688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1324474544"/>
+        <c:axId val="1886701568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,12 +433,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324470448"/>
+        <c:crossAx val="1886704688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1324470448"/>
+        <c:axId val="1886704688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -550,7 +550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324474544"/>
+        <c:crossAx val="1886701568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -786,11 +786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1324442512"/>
-        <c:axId val="-1324404688"/>
+        <c:axId val="1881880864"/>
+        <c:axId val="1881884208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1324442512"/>
+        <c:axId val="1881880864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,12 +902,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324404688"/>
+        <c:crossAx val="1881884208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1324404688"/>
+        <c:axId val="1881884208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1019,7 +1019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324442512"/>
+        <c:crossAx val="1881880864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2510,7 +2510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>

</xml_diff>